<commit_message>
released pgp email onlu unused
</commit_message>
<xml_diff>
--- a/uploads/import_pgp_emails (1).xlsx
+++ b/uploads/import_pgp_emails (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usman\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,31 +24,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="2">
   <si>
     <t>pgp_email</t>
   </si>
   <si>
     <t>example@domain.com</t>
   </si>
-  <si>
-    <t>example1</t>
-  </si>
-  <si>
-    <t>example1@domain.com</t>
-  </si>
-  <si>
-    <t>example2@domain.com</t>
-  </si>
-  <si>
-    <t>1619DKV@ARMORSEC.XYZ</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,12 +51,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF545454"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,10 +74,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -377,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,16 +378,18 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -436,25 +419,13 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A3:A11" r:id="rId2" display="example@domain.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>